<commit_message>
added serial time measurements
</commit_message>
<xml_diff>
--- a/time_measurements.xlsx
+++ b/time_measurements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="11">
   <si>
     <t>number of threads</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Number of Threads</t>
+  </si>
+  <si>
+    <t>Serial 64:</t>
+  </si>
+  <si>
+    <t>Avg</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1655,6 +1661,71 @@
         <v>2.6847672144764849</v>
       </c>
     </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5.1800000000000001E-4</v>
+      </c>
+      <c r="B26">
+        <f>(A26+A27+A28)/3</f>
+        <v>5.3066666666666659E-4</v>
+      </c>
+      <c r="F26">
+        <v>2.4167999999999999E-2</v>
+      </c>
+      <c r="G26">
+        <f>(F26+F27+F28)/3</f>
+        <v>2.4093333333333331E-2</v>
+      </c>
+      <c r="K26">
+        <v>1.420498</v>
+      </c>
+      <c r="L26">
+        <f>(K26+K27+K28)/3</f>
+        <v>1.4208756666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5.1699999999999999E-4</v>
+      </c>
+      <c r="F27">
+        <v>2.402E-2</v>
+      </c>
+      <c r="K27">
+        <v>1.421127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5.5699999999999999E-4</v>
+      </c>
+      <c r="F28">
+        <v>2.4091999999999999E-2</v>
+      </c>
+      <c r="K28">
+        <v>1.4210020000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>